<commit_message>
Comiting with final changes
</commit_message>
<xml_diff>
--- a/Framework/TestData/TestData.xlsx
+++ b/Framework/TestData/TestData.xlsx
@@ -3,19 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rchandr7\eclipse-workspace\Framework\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFF6E37-1B76-4D66-A021-E37BC33939F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CB38FC99-6206-4A09-B82A-9F05C141CFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="804" windowWidth="23040" windowHeight="12504" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Hours" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:P5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -350,7 +347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -367,4 +364,36 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755FC375-3CD4-44F2-8827-C80085F46108}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
+      <c r="C1">
+        <v>8</v>
+      </c>
+      <c r="D1">
+        <v>8</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>